<commit_message>
Complemento do Dicionário de dados
</commit_message>
<xml_diff>
--- a/documents/xlsx/Dicionário de dados.xlsx
+++ b/documents/xlsx/Dicionário de dados.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dicionario dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Dicionario de entidades" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="90">
   <si>
     <t xml:space="preserve">Entidade: bd_nig.tb_empresa </t>
   </si>
@@ -252,6 +253,48 @@
   </si>
   <si>
     <t>Numérico decimal real</t>
+  </si>
+  <si>
+    <t>Entidade</t>
+  </si>
+  <si>
+    <t>Nome da tabela</t>
+  </si>
+  <si>
+    <t>Volume esperado</t>
+  </si>
+  <si>
+    <t>Tempo de retenção</t>
+  </si>
+  <si>
+    <t>Rotina de limpeza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bd_nig.tb_empresa </t>
+  </si>
+  <si>
+    <t>Permanente</t>
+  </si>
+  <si>
+    <t>Não se aplica</t>
+  </si>
+  <si>
+    <t>Carga inicial de 20 ocorrências e volume semanal de 4 ocorrências.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidade responsável por armazenar os dados das empresas que contratarem o sistema de monitoramento. </t>
+  </si>
+  <si>
+    <t>Carga inicial de 60 ocorrências e volume semanal de 10 ocorrências.</t>
+  </si>
+  <si>
+    <t>Temporário</t>
+  </si>
+  <si>
+    <t>A cada 6 meses</t>
+  </si>
+  <si>
+    <t>A cada 12 meses</t>
   </si>
 </sst>
 </file>
@@ -392,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -404,6 +447,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -423,55 +517,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,44 +837,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,14 +891,14 @@
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -849,14 +916,14 @@
       <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -874,14 +941,14 @@
       <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -899,14 +966,14 @@
       <c r="E6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -924,14 +991,14 @@
       <c r="E7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -949,80 +1016,80 @@
       <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1036,12 +1103,12 @@
       <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1057,12 +1124,12 @@
       <c r="E14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1078,12 +1145,12 @@
       <c r="E15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1099,12 +1166,12 @@
       <c r="E16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1120,12 +1187,12 @@
       <c r="E17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -1141,12 +1208,12 @@
       <c r="E18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1162,12 +1229,12 @@
       <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1183,12 +1250,12 @@
       <c r="E20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1204,12 +1271,12 @@
       <c r="E21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1223,52 +1290,52 @@
       <c r="E22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="14"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="16"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -1282,12 +1349,12 @@
       <c r="E27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1301,12 +1368,12 @@
       <c r="E28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1320,12 +1387,12 @@
       <c r="E29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1341,12 +1408,12 @@
       <c r="E30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -1360,52 +1427,52 @@
       <c r="E31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-    </row>
-    <row r="35" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+    </row>
+    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="16"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1419,12 +1486,12 @@
       <c r="E36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -1440,12 +1507,12 @@
       <c r="E37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -1459,78 +1526,78 @@
       <c r="E38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="14"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="16"/>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -1544,12 +1611,12 @@
       <c r="E43" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -1563,12 +1630,12 @@
       <c r="E44" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -1584,12 +1651,12 @@
       <c r="E45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="19"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="21"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="12"/>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -1603,65 +1670,65 @@
       <c r="E46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="27"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="19"/>
     </row>
     <row r="50" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="14"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="16"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -1675,12 +1742,12 @@
       <c r="E51" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F51" s="19"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="21"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="12"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
@@ -1696,12 +1763,12 @@
       <c r="E52" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="12"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -1715,12 +1782,12 @@
       <c r="E53" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -1734,12 +1801,12 @@
       <c r="E54" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="21"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="12"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1753,12 +1820,12 @@
       <c r="E55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="21"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="12"/>
     </row>
     <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
@@ -1772,52 +1839,52 @@
       <c r="E56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
     </row>
     <row r="59" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="14"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="16"/>
     </row>
     <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -1831,12 +1898,12 @@
       <c r="E61" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
@@ -1852,12 +1919,12 @@
       <c r="E62" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="21"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="12"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
@@ -1871,12 +1938,12 @@
       <c r="E63" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
     </row>
     <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
@@ -1890,52 +1957,52 @@
       <c r="E64" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
     </row>
     <row r="67" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D68" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="E68" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="14"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="16"/>
     </row>
     <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
@@ -1949,12 +2016,12 @@
       <c r="E69" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
@@ -1968,12 +2035,12 @@
       <c r="E70" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F70" s="19"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="21"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="12"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
@@ -1987,12 +2054,12 @@
       <c r="E71" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
     </row>
     <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
@@ -2006,15 +2073,58 @@
       <c r="E72" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="A9:K10"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="F37:K37"/>
+    <mergeCell ref="F61:K61"/>
+    <mergeCell ref="F62:K62"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="F53:K53"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="F44:K44"/>
     <mergeCell ref="F46:K46"/>
     <mergeCell ref="F45:K45"/>
     <mergeCell ref="F71:K71"/>
@@ -2031,51 +2141,185 @@
     <mergeCell ref="F52:K52"/>
     <mergeCell ref="A59:K59"/>
     <mergeCell ref="F60:K60"/>
-    <mergeCell ref="F61:K61"/>
-    <mergeCell ref="F62:K62"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="F50:K50"/>
-    <mergeCell ref="F51:K51"/>
-    <mergeCell ref="F53:K53"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="F42:K42"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="F44:K44"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="F37:K37"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="F12:K12"/>
-    <mergeCell ref="A9:K10"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F8:K8"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes no script do banco de dados, tabelas de dados unificadas e retirei o codigo da empresa da table empresa. Atualizei o MER.
</commit_message>
<xml_diff>
--- a/documents/xlsx/Dicionário de dados.xlsx
+++ b/documents/xlsx/Dicionário de dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario dados" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="157">
   <si>
     <t xml:space="preserve">Entidade: bd_nig.tb_empresa </t>
   </si>
@@ -327,9 +327,6 @@
     <t>Carga inicial de 60 ocorrências e volume semanal de 160 ocorrências.</t>
   </si>
   <si>
-    <t>Carga inicial de 96 ocorrências e volume semanal de 96 ocorrências.</t>
-  </si>
-  <si>
     <t>Sobrenome do funcionário.</t>
   </si>
   <si>
@@ -493,6 +490,12 @@
   </si>
   <si>
     <t>Chave estrangeira e relacionamento com a tabela área para que cada microcontrolador tenha obrigatoriamente uma área cadastrada na sua localização.</t>
+  </si>
+  <si>
+    <t>Carga inicial de 0 ocorrências e volume semanal de 672 ocorrências semanais.</t>
+  </si>
+  <si>
+    <t>(ESTAMOS VERIFICANDO SE CONSEGUIMOS PUXAR O IP DO COMPUTADOR DE ONDE O USUARIO ESTA FAZENDO O LOGIN)</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -690,6 +693,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,65 +765,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:K56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,19 +1065,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1089,14 +1095,14 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1110,19 +1116,19 @@
         <v>25</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1140,14 +1146,14 @@
       <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1165,14 +1171,14 @@
       <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1190,14 +1196,14 @@
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1215,14 +1221,14 @@
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="37"/>
+      <c r="F7" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1240,55 +1246,55 @@
       <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="28"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1306,18 +1312,18 @@
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
     </row>
     <row r="13" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
@@ -1326,23 +1332,23 @@
         <v>25</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="37"/>
+      <c r="F13" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
@@ -1356,18 +1362,18 @@
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
+      <c r="F14" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>30</v>
@@ -1381,18 +1387,18 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="F15" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -1406,18 +1412,18 @@
       <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
+      <c r="F16" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1431,18 +1437,18 @@
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
+      <c r="F17" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
@@ -1456,24 +1462,24 @@
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="F18" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -1481,18 +1487,18 @@
       <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
+      <c r="F19" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>35</v>
@@ -1506,18 +1512,18 @@
       <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
+      <c r="F20" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>36</v>
@@ -1531,18 +1537,18 @@
       <c r="E21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
+      <c r="F21" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>37</v>
@@ -1551,34 +1557,34 @@
         <v>25</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
+      <c r="F22" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="25" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1596,18 +1602,18 @@
       <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="30"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>41</v>
@@ -1616,23 +1622,23 @@
         <v>25</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="28"/>
+      <c r="F27" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>42</v>
@@ -1641,23 +1647,23 @@
         <v>46</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
+      <c r="F28" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>43</v>
@@ -1666,44 +1672,46 @@
         <v>46</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39" t="s">
+      <c r="F29" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+    </row>
+    <row r="30" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="19">
         <v>15</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
+      <c r="F30" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>45</v>
@@ -1712,34 +1720,34 @@
         <v>25</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
+      <c r="F31" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1757,18 +1765,18 @@
       <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="25"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>48</v>
@@ -1777,23 +1785,23 @@
         <v>25</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="28"/>
+      <c r="F36" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>49</v>
@@ -1807,18 +1815,18 @@
       <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
+      <c r="F37" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
@@ -1827,19 +1835,19 @@
         <v>25</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
+      <c r="F38" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="34"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
@@ -1868,19 +1876,19 @@
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1898,18 +1906,18 @@
       <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="30"/>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>51</v>
@@ -1918,23 +1926,23 @@
         <v>25</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="28"/>
+      <c r="F43" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="26"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>52</v>
@@ -1943,23 +1951,23 @@
         <v>25</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="F44" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
     </row>
     <row r="45" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>53</v>
@@ -1973,18 +1981,18 @@
       <c r="E45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="28"/>
+      <c r="F45" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="26"/>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>54</v>
@@ -1993,19 +2001,19 @@
         <v>25</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
+      <c r="F46" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
@@ -2021,19 +2029,19 @@
       <c r="K47" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="31"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="37"/>
     </row>
     <row r="50" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2051,18 +2059,18 @@
       <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F50" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="25"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="30"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>59</v>
@@ -2071,23 +2079,23 @@
         <v>25</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="28"/>
+      <c r="F51" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="26"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>60</v>
@@ -2101,16 +2109,16 @@
       <c r="E52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="41"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>61</v>
@@ -2119,21 +2127,21 @@
         <v>71</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>62</v>
@@ -2142,21 +2150,21 @@
         <v>71</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="21"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="41"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>63</v>
@@ -2165,21 +2173,21 @@
         <v>72</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="21"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="41"/>
     </row>
     <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>64</v>
@@ -2188,32 +2196,32 @@
         <v>25</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
     </row>
     <row r="59" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="27"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2231,18 +2239,18 @@
       <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="23" t="s">
+      <c r="F60" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="25"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="30"/>
     </row>
     <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>65</v>
@@ -2251,23 +2259,23 @@
         <v>25</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="28"/>
+      <c r="F61" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="26"/>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>66</v>
@@ -2281,16 +2289,16 @@
       <c r="E62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="21"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="41"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>67</v>
@@ -2299,21 +2307,21 @@
         <v>71</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
     </row>
     <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>68</v>
@@ -2322,32 +2330,32 @@
         <v>25</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
     </row>
     <row r="67" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
     </row>
     <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
@@ -2365,18 +2373,18 @@
       <c r="E68" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F68" s="23" t="s">
+      <c r="F68" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-      <c r="K68" s="25"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="30"/>
     </row>
     <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>69</v>
@@ -2385,23 +2393,23 @@
         <v>25</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F69" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="28"/>
+      <c r="F69" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="26"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>70</v>
@@ -2410,21 +2418,21 @@
         <v>25</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F70" s="19"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="21"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="40"/>
+      <c r="H70" s="40"/>
+      <c r="I70" s="40"/>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>67</v>
@@ -2433,21 +2441,21 @@
         <v>71</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
     </row>
     <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>68</v>
@@ -2456,64 +2464,20 @@
         <v>25</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F8:K8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="F12:K12"/>
-    <mergeCell ref="A9:K10"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="F37:K37"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="F50:K50"/>
-    <mergeCell ref="F51:K51"/>
-    <mergeCell ref="F53:K53"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="F42:K42"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="F44:K44"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="F45:K45"/>
-    <mergeCell ref="F52:K52"/>
     <mergeCell ref="F71:K71"/>
     <mergeCell ref="F72:K72"/>
     <mergeCell ref="F55:K55"/>
@@ -2529,6 +2493,50 @@
     <mergeCell ref="F60:K60"/>
     <mergeCell ref="F61:K61"/>
     <mergeCell ref="F62:K62"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="F53:K53"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="F44:K44"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="F45:K45"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="F37:K37"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="A9:K10"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="F6:K6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2539,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2701,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>57</v>
       </c>
@@ -2704,7 +2712,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>86</v>
@@ -2713,7 +2721,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>58</v>
       </c>
@@ -2724,7 +2732,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>86</v>
@@ -2735,5 +2743,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalização do Dicionario de dados com as sugestões da professora Célia
</commit_message>
<xml_diff>
--- a/documents/xlsx/Dicionário de dados.xlsx
+++ b/documents/xlsx/Dicionário de dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario dados" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="161">
   <si>
     <t xml:space="preserve">Entidade: bd_nig.tb_empresa </t>
   </si>
@@ -198,12 +198,6 @@
     <t>bd_nig.tb_sensor_dht11</t>
   </si>
   <si>
-    <t>bd_nig.tb_dado_temperatura</t>
-  </si>
-  <si>
-    <t>bd_nig.tb_dado_umidade</t>
-  </si>
-  <si>
     <t>id_sensor_dht11</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>fk_sensor</t>
   </si>
   <si>
-    <t>id_umidade</t>
-  </si>
-  <si>
     <t>umidade</t>
   </si>
   <si>
@@ -297,15 +288,6 @@
     <t>Entidade responsável por armazenar os dados dos funcionários responsáveis por gerenciar o sistema das empresas contratantes.</t>
   </si>
   <si>
-    <t>Entidade responsável por armazenar os dados de login/logout dos funcionários no sistema.</t>
-  </si>
-  <si>
-    <t>Entidade responsável por armazenar os dados coletados do sensor referente a umidade.</t>
-  </si>
-  <si>
-    <t>Entidade responsável por armazenar os dados coletados do sensor referente a temperatura.</t>
-  </si>
-  <si>
     <t>Entidade responsável por armazenar os dados referente as áreas, em uma visão macro,  onde os sensores serão instalados.</t>
   </si>
   <si>
@@ -357,9 +339,6 @@
     <t>Id de identificação única e relacionamento no banco de dados do funcionário.</t>
   </si>
   <si>
-    <t>s/limite</t>
-  </si>
-  <si>
     <t>Id de identificação e relacionamento no banco de dados do login no sistema.</t>
   </si>
   <si>
@@ -414,9 +393,6 @@
     <t>Id de identificação e relacionamento no banco de dados da temperatura.</t>
   </si>
   <si>
-    <t>Id de identificação e relacionamento no banco de dados da umidade.</t>
-  </si>
-  <si>
     <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_empresa e tb_controle_login.</t>
   </si>
   <si>
@@ -429,9 +405,6 @@
     <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_area e tb_sensor_dht11.</t>
   </si>
   <si>
-    <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_sensor_dht11 e tb_temperatura e tb_umidade.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primeiro nome do funcionário. </t>
   </si>
   <si>
@@ -492,10 +465,49 @@
     <t>Chave estrangeira e relacionamento com a tabela área para que cada microcontrolador tenha obrigatoriamente uma área cadastrada na sua localização.</t>
   </si>
   <si>
-    <t>Carga inicial de 0 ocorrências e volume semanal de 672 ocorrências semanais.</t>
-  </si>
-  <si>
     <t>(ESTAMOS VERIFICANDO SE CONSEGUIMOS PUXAR O IP DO COMPUTADOR DE ONDE O USUARIO ESTA FAZENDO O LOGIN)</t>
+  </si>
+  <si>
+    <t>bd_nig.tb_dado_dht11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O campo irá armazenar os registros da umidade coletada através do sensor DHT11. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O campo irá armazenar os registros da temperatura coletada através do sensor DHT11 na formatação 00,0. </t>
+  </si>
+  <si>
+    <t>Campo deverá coletar o horário em que o dado foi captado e registrado pelo sensor DHT11, no formato hh:mm:ss.</t>
+  </si>
+  <si>
+    <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_sensor_dht11 e tb_dado_dht11.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira e relacionamento com a tabela sensor para que cada dado de temperatura e umidade sejam obrigatoriamente relacionados a um sensor de captação.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira e relacionamento com a tabela dados_dht11 e microcontrolador para que cada sensor de temperatura e umidade estejam obrigatoriamente relacionados a uma área exata e registrar os dados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do sensor, sem formatação pré-definida. </t>
+  </si>
+  <si>
+    <t>Data do ínicio do funcionamento do sensor, contando com 2 digitos do dia, 2 digitos do mês e 4 digitos do ano.</t>
+  </si>
+  <si>
+    <t>Data do término do funcionamento do sensor, contando com 2 digitos do dia, 2 digitos do mês e 4 digitos do ano.</t>
+  </si>
+  <si>
+    <t>Campo onde irá armazenar o digito booleano do sensor, verificando se está ativo (1) ou desligado (0).</t>
+  </si>
+  <si>
+    <t>Entidade responsável por armazenar os dados de login/logout dos funcionários no sistema. Limpeza de todos os dados da entidade a cada 6 meses, gerando um histórico em PDF antes da limpeza para arquivo.</t>
+  </si>
+  <si>
+    <t>Entidade responsável por armazenar os dados coletados do sensor referente a temperatura e a umidade.  Limpeza de todos os dados da entidade a cada 12 meses, gerando um histórico em PDF antes da limpeza para arquivo.</t>
+  </si>
+  <si>
+    <t>Carga inicial de 0 ocorrências e volume semanal de 1.344 ocorrências semanais.</t>
   </si>
 </sst>
 </file>
@@ -657,15 +669,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,6 +705,57 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -712,61 +766,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,19 +1077,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1095,14 +1107,14 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1115,20 +1127,20 @@
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>110</v>
+      <c r="D3" s="6">
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1221,14 +1233,14 @@
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
+      <c r="F7" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1256,45 +1268,45 @@
       <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1312,18 +1324,18 @@
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>109</v>
+      <c r="A13" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
@@ -1331,24 +1343,24 @@
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>110</v>
+      <c r="D13" s="3">
+        <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
+      <c r="F13" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
@@ -1363,7 +1375,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
@@ -1373,7 +1385,7 @@
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>30</v>
@@ -1387,18 +1399,18 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="F15" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -1413,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
@@ -1423,7 +1435,7 @@
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1438,7 +1450,7 @@
         <v>39</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -1448,7 +1460,7 @@
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
@@ -1462,24 +1474,24 @@
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
+      <c r="F18" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -1488,7 +1500,7 @@
         <v>23</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
@@ -1498,7 +1510,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>35</v>
@@ -1512,18 +1524,18 @@
       <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
+      <c r="F20" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>36</v>
@@ -1538,7 +1550,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
@@ -1547,8 +1559,8 @@
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>107</v>
+      <c r="A22" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>37</v>
@@ -1556,35 +1568,61 @@
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>110</v>
+      <c r="D22" s="6">
+        <v>4</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="F22" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1602,18 +1640,18 @@
       <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="30"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>111</v>
+      <c r="A27" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>41</v>
@@ -1621,14 +1659,14 @@
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>110</v>
+      <c r="D27" s="6">
+        <v>4</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
@@ -1638,7 +1676,7 @@
     </row>
     <row r="28" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>42</v>
@@ -1646,24 +1684,24 @@
       <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>110</v>
+      <c r="D28" s="6">
+        <v>8</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
+      <c r="F28" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>43</v>
@@ -1671,47 +1709,47 @@
       <c r="C29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>110</v>
+      <c r="D29" s="6">
+        <v>8</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
+      <c r="F29" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
     </row>
     <row r="30" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="16">
         <v>15</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
+      <c r="F30" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>108</v>
+      <c r="A31" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>45</v>
@@ -1719,35 +1757,61 @@
       <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>110</v>
+      <c r="D31" s="6">
+        <v>4</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
+      <c r="F31" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1765,18 +1829,18 @@
       <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="30"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>114</v>
+      <c r="A36" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>48</v>
@@ -1784,14 +1848,14 @@
       <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>110</v>
+      <c r="D36" s="6">
+        <v>4</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
@@ -1801,7 +1865,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>49</v>
@@ -1815,18 +1879,18 @@
       <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
+      <c r="F37" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>107</v>
+      <c r="A38" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
@@ -1834,61 +1898,61 @@
       <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>110</v>
+      <c r="D38" s="6">
+        <v>4</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
+      <c r="F38" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1906,18 +1970,18 @@
       <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="30"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>118</v>
+      <c r="A43" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>51</v>
@@ -1925,14 +1989,14 @@
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>110</v>
+      <c r="D43" s="6">
+        <v>4</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
@@ -1942,7 +2006,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>52</v>
@@ -1950,14 +2014,14 @@
       <c r="C44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>110</v>
+      <c r="D44" s="6">
+        <v>4</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F44" s="31" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -1967,7 +2031,7 @@
     </row>
     <row r="45" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>53</v>
@@ -1982,7 +2046,7 @@
         <v>23</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G45" s="25"/>
       <c r="H45" s="25"/>
@@ -1991,8 +2055,8 @@
       <c r="K45" s="26"/>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>114</v>
+      <c r="A46" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>54</v>
@@ -2000,48 +2064,61 @@
       <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>110</v>
+      <c r="D46" s="6">
+        <v>4</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
+      <c r="F46" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="42"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
     </row>
     <row r="49" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="37"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2059,33 +2136,33 @@
       <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="28" t="s">
+      <c r="F50" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="30"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>126</v>
+      <c r="A51" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>110</v>
+      <c r="D51" s="6">
+        <v>4</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G51" s="25"/>
       <c r="H51" s="25"/>
@@ -2095,10 +2172,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>17</v>
@@ -2109,119 +2186,155 @@
       <c r="E52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="41"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F52" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="40"/>
+    </row>
+    <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>110</v>
+        <v>68</v>
+      </c>
+      <c r="D53" s="6">
+        <v>8</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F53" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+    </row>
+    <row r="54" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>110</v>
+        <v>68</v>
+      </c>
+      <c r="D54" s="6">
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="39"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="41"/>
+      <c r="F54" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>110</v>
+        <v>69</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" s="39"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="41"/>
+        <v>70</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>127</v>
+      <c r="A56" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>110</v>
+      <c r="D56" s="6">
+        <v>4</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="38"/>
-      <c r="J56" s="38"/>
-      <c r="K56" s="38"/>
+      <c r="F56" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
     </row>
     <row r="59" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="27"/>
+      <c r="A59" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2239,33 +2352,33 @@
       <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="28" t="s">
+      <c r="F60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="30"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="23"/>
     </row>
     <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>128</v>
+      <c r="A61" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>110</v>
+      <c r="D61" s="6">
+        <v>4</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
@@ -2275,13 +2388,13 @@
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="D62" s="3">
         <v>3.1</v>
@@ -2289,210 +2402,128 @@
       <c r="E62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="39"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="40"/>
-      <c r="K62" s="41"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F62" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>110</v>
+      <c r="C63" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="19">
+        <v>4</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="38"/>
-      <c r="K63" s="38"/>
-    </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>126</v>
+      <c r="F63" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="40"/>
+    </row>
+    <row r="64" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="6">
+        <v>8</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+    </row>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64" s="4" t="s">
+      <c r="D65" s="6">
+        <v>4</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F64" s="38"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-    </row>
-    <row r="67" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-    </row>
-    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="30"/>
-    </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
-      <c r="I69" s="25"/>
-      <c r="J69" s="25"/>
-      <c r="K69" s="26"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="39"/>
-      <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
-      <c r="J70" s="40"/>
-      <c r="K70" s="41"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="38"/>
-    </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F72" s="38"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="38"/>
-      <c r="J72" s="38"/>
-      <c r="K72" s="38"/>
-    </row>
+      <c r="F65" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="26"/>
+    </row>
+    <row r="70" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F71:K71"/>
-    <mergeCell ref="F72:K72"/>
-    <mergeCell ref="F55:K55"/>
-    <mergeCell ref="F54:K54"/>
-    <mergeCell ref="F63:K63"/>
-    <mergeCell ref="F64:K64"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="F68:K68"/>
-    <mergeCell ref="F69:K69"/>
-    <mergeCell ref="F70:K70"/>
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="F60:K60"/>
-    <mergeCell ref="F61:K61"/>
-    <mergeCell ref="F62:K62"/>
+    <mergeCell ref="A57:K58"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="A9:K10"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="A23:K24"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="F37:K37"/>
+    <mergeCell ref="A32:K33"/>
     <mergeCell ref="F38:K38"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="F50:K50"/>
@@ -2505,38 +2536,18 @@
     <mergeCell ref="F46:K46"/>
     <mergeCell ref="F45:K45"/>
     <mergeCell ref="F52:K52"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="F37:K37"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="F12:K12"/>
-    <mergeCell ref="A9:K10"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F8:K8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="A39:K40"/>
+    <mergeCell ref="A47:K48"/>
+    <mergeCell ref="F55:K55"/>
+    <mergeCell ref="F54:K54"/>
+    <mergeCell ref="F64:K64"/>
+    <mergeCell ref="F65:K65"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="F60:K60"/>
+    <mergeCell ref="F61:K61"/>
+    <mergeCell ref="F62:K62"/>
+    <mergeCell ref="F63:K63"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2545,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,183 +2573,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="14" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="F8" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção na planilha do dicionário de dados
</commit_message>
<xml_diff>
--- a/documents/xlsx/Dicionário de dados.xlsx
+++ b/documents/xlsx/Dicionário de dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario dados" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="161">
   <si>
     <t xml:space="preserve">Entidade: bd_nig.tb_empresa </t>
   </si>
@@ -198,12 +198,6 @@
     <t>bd_nig.tb_sensor_dht11</t>
   </si>
   <si>
-    <t>bd_nig.tb_dado_temperatura</t>
-  </si>
-  <si>
-    <t>bd_nig.tb_dado_umidade</t>
-  </si>
-  <si>
     <t>id_sensor_dht11</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>fk_sensor</t>
   </si>
   <si>
-    <t>id_umidade</t>
-  </si>
-  <si>
     <t>umidade</t>
   </si>
   <si>
@@ -297,15 +288,6 @@
     <t>Entidade responsável por armazenar os dados dos funcionários responsáveis por gerenciar o sistema das empresas contratantes.</t>
   </si>
   <si>
-    <t>Entidade responsável por armazenar os dados de login/logout dos funcionários no sistema.</t>
-  </si>
-  <si>
-    <t>Entidade responsável por armazenar os dados coletados do sensor referente a umidade.</t>
-  </si>
-  <si>
-    <t>Entidade responsável por armazenar os dados coletados do sensor referente a temperatura.</t>
-  </si>
-  <si>
     <t>Entidade responsável por armazenar os dados referente as áreas, em uma visão macro,  onde os sensores serão instalados.</t>
   </si>
   <si>
@@ -327,9 +309,6 @@
     <t>Carga inicial de 60 ocorrências e volume semanal de 160 ocorrências.</t>
   </si>
   <si>
-    <t>Carga inicial de 96 ocorrências e volume semanal de 96 ocorrências.</t>
-  </si>
-  <si>
     <t>Sobrenome do funcionário.</t>
   </si>
   <si>
@@ -360,9 +339,6 @@
     <t>Id de identificação única e relacionamento no banco de dados do funcionário.</t>
   </si>
   <si>
-    <t>s/limite</t>
-  </si>
-  <si>
     <t>Id de identificação e relacionamento no banco de dados do login no sistema.</t>
   </si>
   <si>
@@ -417,9 +393,6 @@
     <t>Id de identificação e relacionamento no banco de dados da temperatura.</t>
   </si>
   <si>
-    <t>Id de identificação e relacionamento no banco de dados da umidade.</t>
-  </si>
-  <si>
     <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_empresa e tb_controle_login.</t>
   </si>
   <si>
@@ -432,9 +405,6 @@
     <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_area e tb_sensor_dht11.</t>
   </si>
   <si>
-    <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_sensor_dht11 e tb_temperatura e tb_umidade.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primeiro nome do funcionário. </t>
   </si>
   <si>
@@ -493,6 +463,51 @@
   </si>
   <si>
     <t>Chave estrangeira e relacionamento com a tabela área para que cada microcontrolador tenha obrigatoriamente uma área cadastrada na sua localização.</t>
+  </si>
+  <si>
+    <t>(ESTAMOS VERIFICANDO SE CONSEGUIMOS PUXAR O IP DO COMPUTADOR DE ONDE O USUARIO ESTA FAZENDO O LOGIN)</t>
+  </si>
+  <si>
+    <t>bd_nig.tb_dado_dht11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O campo irá armazenar os registros da umidade coletada através do sensor DHT11. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O campo irá armazenar os registros da temperatura coletada através do sensor DHT11 na formatação 00,0. </t>
+  </si>
+  <si>
+    <t>Campo deverá coletar o horário em que o dado foi captado e registrado pelo sensor DHT11, no formato hh:mm:ss.</t>
+  </si>
+  <si>
+    <t>O id será para identificar a tabela e fazer o relacionamento com as entidades tb_sensor_dht11 e tb_dado_dht11.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira e relacionamento com a tabela sensor para que cada dado de temperatura e umidade sejam obrigatoriamente relacionados a um sensor de captação.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira e relacionamento com a tabela dados_dht11 e microcontrolador para que cada sensor de temperatura e umidade estejam obrigatoriamente relacionados a uma área exata e registrar os dados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do sensor, sem formatação pré-definida. </t>
+  </si>
+  <si>
+    <t>Data do ínicio do funcionamento do sensor, contando com 2 digitos do dia, 2 digitos do mês e 4 digitos do ano.</t>
+  </si>
+  <si>
+    <t>Data do término do funcionamento do sensor, contando com 2 digitos do dia, 2 digitos do mês e 4 digitos do ano.</t>
+  </si>
+  <si>
+    <t>Campo onde irá armazenar o digito booleano do sensor, verificando se está ativo (1) ou desligado (0).</t>
+  </si>
+  <si>
+    <t>Entidade responsável por armazenar os dados de login/logout dos funcionários no sistema. Limpeza de todos os dados da entidade a cada 6 meses, gerando um histórico em PDF antes da limpeza para arquivo.</t>
+  </si>
+  <si>
+    <t>Entidade responsável por armazenar os dados coletados do sensor referente a temperatura e a umidade.  Limpeza de todos os dados da entidade a cada 12 meses, gerando um histórico em PDF antes da limpeza para arquivo.</t>
+  </si>
+  <si>
+    <t>Carga inicial de 0 ocorrências e volume semanal de 1.344 ocorrências semanais.</t>
   </si>
 </sst>
 </file>
@@ -639,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -654,15 +669,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -690,18 +696,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,6 +732,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -735,6 +747,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,17 +765,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:K56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,19 +1077,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1089,14 +1107,14 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1109,8 +1127,8 @@
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>111</v>
+      <c r="D3" s="6">
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>38</v>
@@ -1140,14 +1158,14 @@
       <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1165,14 +1183,14 @@
       <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1190,14 +1208,14 @@
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1216,7 +1234,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
@@ -1240,14 +1258,14 @@
       <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="28"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
@@ -1276,19 +1294,19 @@
       <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1306,18 +1324,18 @@
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>110</v>
+      <c r="A13" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
@@ -1325,14 +1343,14 @@
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>111</v>
+      <c r="D13" s="3">
+        <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
@@ -1342,7 +1360,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
@@ -1356,18 +1374,18 @@
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
+      <c r="F14" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>30</v>
@@ -1381,18 +1399,18 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="F15" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -1406,18 +1424,18 @@
       <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
+      <c r="F16" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1431,18 +1449,18 @@
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
+      <c r="F17" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
@@ -1456,24 +1474,24 @@
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="F18" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -1481,18 +1499,18 @@
       <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
+      <c r="F19" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>35</v>
@@ -1506,18 +1524,18 @@
       <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
+      <c r="F20" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>36</v>
@@ -1531,18 +1549,18 @@
       <c r="E21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
+      <c r="F21" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>108</v>
+      <c r="A22" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>37</v>
@@ -1550,35 +1568,61 @@
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>111</v>
+      <c r="D22" s="6">
+        <v>4</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
+      <c r="F22" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1596,18 +1640,18 @@
       <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>112</v>
+      <c r="A27" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>41</v>
@@ -1615,24 +1659,24 @@
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>111</v>
+      <c r="D27" s="6">
+        <v>4</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="28"/>
+      <c r="F27" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>42</v>
@@ -1640,24 +1684,24 @@
       <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>111</v>
+      <c r="D28" s="6">
+        <v>8</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
+      <c r="F28" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>43</v>
@@ -1665,36 +1709,38 @@
       <c r="C29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>111</v>
+      <c r="D29" s="6">
+        <v>8</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39" t="s">
+      <c r="F29" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="16">
         <v>15</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="32"/>
+      <c r="F30" s="32" t="s">
+        <v>146</v>
+      </c>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
@@ -1702,8 +1748,8 @@
       <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>109</v>
+      <c r="A31" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>45</v>
@@ -1711,35 +1757,61 @@
       <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>111</v>
+      <c r="D31" s="6">
+        <v>4</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
+      <c r="F31" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1757,18 +1829,18 @@
       <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="25"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>115</v>
+      <c r="A36" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>48</v>
@@ -1776,24 +1848,24 @@
       <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>111</v>
+      <c r="D36" s="6">
+        <v>4</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="28"/>
+      <c r="F36" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>49</v>
@@ -1807,18 +1879,18 @@
       <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
+      <c r="F37" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>108</v>
+      <c r="A38" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
@@ -1826,61 +1898,61 @@
       <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>111</v>
+      <c r="D38" s="6">
+        <v>4</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
+      <c r="F38" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1898,18 +1970,18 @@
       <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>119</v>
+      <c r="A43" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>51</v>
@@ -1917,24 +1989,24 @@
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>111</v>
+      <c r="D43" s="6">
+        <v>4</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="28"/>
+      <c r="F43" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="26"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>52</v>
@@ -1942,24 +2014,24 @@
       <c r="C44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>111</v>
+      <c r="D44" s="6">
+        <v>4</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="F44" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
     </row>
     <row r="45" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>53</v>
@@ -1973,18 +2045,18 @@
       <c r="E45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="28"/>
+      <c r="F45" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="26"/>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>115</v>
+      <c r="A46" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>54</v>
@@ -1992,48 +2064,61 @@
       <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>111</v>
+      <c r="D46" s="6">
+        <v>4</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
+      <c r="F46" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="42"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
     </row>
     <row r="49" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="31"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2051,46 +2136,46 @@
       <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F50" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="25"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>127</v>
+      <c r="A51" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>111</v>
+      <c r="D51" s="6">
+        <v>4</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="28"/>
+      <c r="F51" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="26"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>17</v>
@@ -2101,119 +2186,155 @@
       <c r="E52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F52" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="40"/>
+    </row>
+    <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>111</v>
+        <v>68</v>
+      </c>
+      <c r="D53" s="6">
+        <v>8</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F53" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+    </row>
+    <row r="54" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>111</v>
+        <v>68</v>
+      </c>
+      <c r="D54" s="6">
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="21"/>
+      <c r="F54" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>111</v>
+        <v>69</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>128</v>
+      <c r="A56" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>111</v>
+      <c r="D56" s="6">
+        <v>4</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
+      <c r="F56" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
     </row>
     <row r="59" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
+      <c r="A59" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2231,49 +2352,49 @@
       <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="23" t="s">
+      <c r="F60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="25"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="23"/>
     </row>
     <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>129</v>
+      <c r="A61" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>111</v>
+      <c r="D61" s="6">
+        <v>4</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="28"/>
+      <c r="F61" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="26"/>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="D62" s="3">
         <v>3.1</v>
@@ -2281,195 +2402,94 @@
       <c r="E62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="21"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F62" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>111</v>
+      <c r="C63" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="19">
+        <v>4</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-    </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>127</v>
+      <c r="F63" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="40"/>
+    </row>
+    <row r="64" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="6">
+        <v>8</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+    </row>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E64" s="4" t="s">
+      <c r="D65" s="6">
+        <v>4</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-    </row>
-    <row r="67" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
-    </row>
-    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-      <c r="K68" s="25"/>
-    </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="28"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="19"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="21"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18"/>
-    </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-    </row>
+      <c r="F65" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="26"/>
+    </row>
+    <row r="70" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A57:K58"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="F8:K8"/>
     <mergeCell ref="A1:K1"/>
@@ -2497,11 +2517,13 @@
     <mergeCell ref="F27:K27"/>
     <mergeCell ref="F28:K28"/>
     <mergeCell ref="F29:K29"/>
+    <mergeCell ref="A23:K24"/>
     <mergeCell ref="F31:K31"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="F35:K35"/>
     <mergeCell ref="F36:K36"/>
     <mergeCell ref="F37:K37"/>
+    <mergeCell ref="A32:K33"/>
     <mergeCell ref="F38:K38"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="F50:K50"/>
@@ -2514,21 +2536,18 @@
     <mergeCell ref="F46:K46"/>
     <mergeCell ref="F45:K45"/>
     <mergeCell ref="F52:K52"/>
-    <mergeCell ref="F71:K71"/>
-    <mergeCell ref="F72:K72"/>
+    <mergeCell ref="A39:K40"/>
+    <mergeCell ref="A47:K48"/>
     <mergeCell ref="F55:K55"/>
     <mergeCell ref="F54:K54"/>
-    <mergeCell ref="F63:K63"/>
     <mergeCell ref="F64:K64"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="F68:K68"/>
-    <mergeCell ref="F69:K69"/>
-    <mergeCell ref="F70:K70"/>
+    <mergeCell ref="F65:K65"/>
     <mergeCell ref="F56:K56"/>
     <mergeCell ref="A59:K59"/>
     <mergeCell ref="F60:K60"/>
     <mergeCell ref="F61:K61"/>
     <mergeCell ref="F62:K62"/>
+    <mergeCell ref="F63:K63"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2537,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2554,186 +2573,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="14" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="F8" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ata do dia e ajustes no dicionário de dados (tamanho do campo numérico inteiro)
</commit_message>
<xml_diff>
--- a/documents/xlsx/Dicionário de dados.xlsx
+++ b/documents/xlsx/Dicionário de dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario dados" sheetId="1" r:id="rId1"/>
@@ -654,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -711,6 +711,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,18 +747,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,27 +765,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -778,6 +778,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1062,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,19 +1080,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1107,14 +1110,14 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="23"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1127,20 +1130,20 @@
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6">
-        <v>4</v>
+      <c r="D3" s="43">
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1158,14 +1161,14 @@
       <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1183,14 +1186,14 @@
       <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1208,14 +1211,14 @@
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1233,14 +1236,14 @@
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="37"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1258,55 +1261,55 @@
       <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1324,14 +1327,14 @@
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -1343,20 +1346,20 @@
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3">
-        <v>4</v>
+      <c r="D13" s="43">
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="37"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1374,14 +1377,14 @@
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1399,14 +1402,14 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1424,14 +1427,14 @@
       <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1449,14 +1452,14 @@
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1474,14 +1477,14 @@
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1499,14 +1502,14 @@
       <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1524,14 +1527,14 @@
       <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1549,14 +1552,14 @@
       <c r="E21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
@@ -1568,61 +1571,61 @@
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="6">
-        <v>4</v>
+      <c r="D22" s="43">
+        <v>20</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1640,14 +1643,14 @@
       <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="23"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -1659,20 +1662,20 @@
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="6">
-        <v>4</v>
+      <c r="D27" s="43">
+        <v>20</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27"/>
     </row>
     <row r="28" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -1690,14 +1693,14 @@
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
     </row>
     <row r="29" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1715,14 +1718,14 @@
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
     </row>
     <row r="30" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
@@ -1738,14 +1741,14 @@
       <c r="E30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
@@ -1757,61 +1760,61 @@
       <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="6">
-        <v>4</v>
+      <c r="D31" s="43">
+        <v>20</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1829,14 +1832,14 @@
       <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="23"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="31"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
@@ -1848,20 +1851,20 @@
       <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="6">
-        <v>4</v>
+      <c r="D36" s="43">
+        <v>20</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="27"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1879,14 +1882,14 @@
       <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
@@ -1898,20 +1901,20 @@
       <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="6">
-        <v>4</v>
+      <c r="D38" s="43">
+        <v>20</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="27" t="s">
+      <c r="F38" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41"/>
@@ -1940,19 +1943,19 @@
       <c r="K40" s="42"/>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1970,14 +1973,14 @@
       <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="23"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="31"/>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
@@ -1989,20 +1992,20 @@
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="6">
-        <v>4</v>
+      <c r="D43" s="43">
+        <v>20</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="27"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -2020,14 +2023,14 @@
       <c r="E44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -2045,14 +2048,14 @@
       <c r="E45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="27"/>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
@@ -2064,20 +2067,20 @@
       <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="6">
-        <v>4</v>
+      <c r="D46" s="43">
+        <v>20</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="27" t="s">
+      <c r="F46" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41"/>
@@ -2106,19 +2109,19 @@
       <c r="K48" s="42"/>
     </row>
     <row r="49" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="30"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="37"/>
     </row>
     <row r="50" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2136,14 +2139,14 @@
       <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="23"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="31"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
@@ -2155,20 +2158,20 @@
       <c r="C51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="6">
-        <v>4</v>
+      <c r="D51" s="43">
+        <v>20</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="24" t="s">
+      <c r="F51" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="27"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -2211,14 +2214,14 @@
       <c r="E53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="27" t="s">
+      <c r="F53" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
     </row>
     <row r="54" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -2236,14 +2239,14 @@
       <c r="E54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="27" t="s">
+      <c r="F54" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -2280,61 +2283,61 @@
       <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="6">
-        <v>4</v>
+      <c r="D56" s="43">
+        <v>20</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F56" s="24" t="s">
+      <c r="F56" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="27"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
     </row>
     <row r="59" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2352,14 +2355,14 @@
       <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="23"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="31"/>
     </row>
     <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
@@ -2371,20 +2374,20 @@
       <c r="C61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="6">
-        <v>4</v>
+      <c r="D61" s="43">
+        <v>20</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F61" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="25"/>
-      <c r="J61" s="25"/>
-      <c r="K61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="27"/>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -2402,14 +2405,14 @@
       <c r="E62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="24" t="s">
+      <c r="F62" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="27"/>
     </row>
     <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -2422,7 +2425,7 @@
         <v>25</v>
       </c>
       <c r="D63" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>23</v>
@@ -2452,14 +2455,14 @@
       <c r="E64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F64" s="27" t="s">
+      <c r="F64" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
     </row>
     <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
@@ -2471,24 +2474,67 @@
       <c r="C65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D65" s="6">
-        <v>4</v>
+      <c r="D65" s="43">
+        <v>20</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F65" s="24" t="s">
+      <c r="F65" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="25"/>
-      <c r="J65" s="25"/>
-      <c r="K65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="27"/>
     </row>
     <row r="70" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="F55:K55"/>
+    <mergeCell ref="F54:K54"/>
+    <mergeCell ref="F64:K64"/>
+    <mergeCell ref="F65:K65"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="F60:K60"/>
+    <mergeCell ref="F61:K61"/>
+    <mergeCell ref="F62:K62"/>
+    <mergeCell ref="F63:K63"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="F53:K53"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="F44:K44"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="F45:K45"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="A39:K40"/>
+    <mergeCell ref="A47:K48"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="F37:K37"/>
+    <mergeCell ref="A32:K33"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="A23:K24"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
     <mergeCell ref="A57:K58"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="F8:K8"/>
@@ -2505,49 +2551,6 @@
     <mergeCell ref="F13:K13"/>
     <mergeCell ref="F14:K14"/>
     <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="A23:K24"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="F37:K37"/>
-    <mergeCell ref="A32:K33"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="F50:K50"/>
-    <mergeCell ref="F51:K51"/>
-    <mergeCell ref="F53:K53"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="F42:K42"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="F44:K44"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="F45:K45"/>
-    <mergeCell ref="F52:K52"/>
-    <mergeCell ref="A39:K40"/>
-    <mergeCell ref="A47:K48"/>
-    <mergeCell ref="F55:K55"/>
-    <mergeCell ref="F54:K54"/>
-    <mergeCell ref="F64:K64"/>
-    <mergeCell ref="F65:K65"/>
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="F60:K60"/>
-    <mergeCell ref="F61:K61"/>
-    <mergeCell ref="F62:K62"/>
-    <mergeCell ref="F63:K63"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>